<commit_message>
Did tests 1 - 4 Changed confluence.merge function to have a dict instead of if statements, because I am pretty sure we will be adding more -merge-method options in the future.
</commit_message>
<xml_diff>
--- a/tests/test_files/merge_conflict1.xlsx
+++ b/tests/test_files/merge_conflict1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\workspace\confluence\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/Desktop/workspace/confluence/tests/test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73812B5F-324F-462D-8102-D41A13E436FD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25AF9B50-0150-F642-84A5-0D9F78303971}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{423E75E0-199A-4DF2-A619-CEB9F82764E8}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="20740" windowHeight="11160" xr2:uid="{423E75E0-199A-4DF2-A619-CEB9F82764E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,12 +31,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>foo</t>
   </si>
   <si>
     <t>bar</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
   </si>
 </sst>
 </file>
@@ -388,15 +400,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69B08843-1EA5-4AC2-AD39-93423BB5B353}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -404,20 +416,36 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>5</v>
+      <c r="B2" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>6</v>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>